<commit_message>
Add tests for IIUE
</commit_message>
<xml_diff>
--- a/edziennik/tests/test_files/test_2students.xlsx
+++ b/edziennik/tests/test_files/test_2students.xlsx
@@ -176,8 +176,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,98 +209,101 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>690506333</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>77722233</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="n">
+        <v>777222333</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>